<commit_message>
Check line 150 next
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298241AB-5372-452F-A2F9-7EB11660D526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC6F4C-0C80-4E91-9DD2-8FDF67C4234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11244" yWindow="3492" windowWidth="10884" windowHeight="9504" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="-24420" yWindow="1968" windowWidth="22344" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="12">
   <si>
     <t>Kanal</t>
   </si>
@@ -67,17 +67,7 @@
     <t>This is a test Text</t>
   </si>
   <si>
-    <t>yyyyyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. In porttitor ligula ac turpis eleifend blandit. In elementum velit quis turpis lobortis finibus. Morbi ex dui, facilisis sed mattis ut, vulputate ac odio. Ut rhoncus, quam sed accumsan tempor, purus felis egestas quam, quis pulvinar libero justo at sem. Fusce ac volutpat sapien. Vestibulum pretium ullamcorper fermentum. Mauris vitae eleifend dolor. Sed vel neque et enim ornare consequat. In nec placerat metus. Duis feugiat tellus vel justo faucibus euismod. </t>
-  </si>
-  <si>
-    <t>&lt;!DOCTYPE HTML PUBLIC "-//W3C//DTD HTML 4.0//EN" "http://www.w3.org/TR/REC-html40/strict.dtd"&gt;
-&lt;html&gt;&lt;head&gt;&lt;meta name="qrichtext" content="1" /&gt;&lt;style type="text/css"&gt;
-p, li { white-space: pre-wrap; }
-&lt;/style&gt;&lt;/head&gt;&lt;body style=" font-family:'MS Shell Dlg 2'; font-size:10pt; font-weight:400; font-style:normal;"&gt;
-&lt;p align="right" style=" margin-top:0px; margin-bottom:0px; margin-left:0px; margin-right:0px; -qt-block-indent:0; text-indent:0px;"&gt;Lorem ipsum dolor sit amet, consectetur &lt;span style=" background-color:#447eed;"&gt;adipiscing elit&lt;/span&gt;. In porttitor ligula ac turpis eleifend blandit.&lt;/p&gt;&lt;/body&gt;&lt;/html&gt;</t>
+    <t>T2A gerechtfertigt?</t>
   </si>
 </sst>
 </file>
@@ -440,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
-  <dimension ref="A1:G536"/>
+  <dimension ref="A1:H536"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +446,7 @@
     <col min="7" max="7" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +468,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -492,17 +485,10 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -512,11 +498,9 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -527,7 +511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -538,7 +522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -549,7 +533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -560,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -571,7 +555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -582,7 +566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -593,7 +577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -604,7 +588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -615,7 +599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -626,7 +610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -637,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -648,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Chat loading and scraping complete
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC6F4C-0C80-4E91-9DD2-8FDF67C4234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC78386-FB16-41A1-8F51-FB67BD934FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24420" yWindow="1968" windowWidth="22344" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="12">
   <si>
     <t>Kanal</t>
   </si>
@@ -64,20 +64,28 @@
     <t>11111-D11111111110000</t>
   </si>
   <si>
-    <t>This is a test Text</t>
+    <t>T2A gerechtfertigt?</t>
   </si>
   <si>
-    <t>T2A gerechtfertigt?</t>
+    <t>https://www.cleverbot.com/conv/202202041647/WYDS891QFL_Hello-who-are-you</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,18 +114,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,15 +444,15 @@
   <dimension ref="A1:H536"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E2" sqref="E2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="69.77734375" customWidth="1"/>
     <col min="5" max="6" width="21.77734375" customWidth="1"/>
     <col min="7" max="7" width="29.21875" customWidth="1"/>
   </cols>
@@ -469,7 +480,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -482,13 +493,13 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -498,6 +509,10 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -510,6 +525,11 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -521,6 +541,11 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -532,6 +557,12 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -543,6 +574,9 @@
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -554,6 +588,9 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -565,6 +602,9 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -576,6 +616,9 @@
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -587,6 +630,9 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -598,6 +644,9 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -609,6 +658,9 @@
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -620,6 +672,9 @@
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -631,6 +686,9 @@
       <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -642,8 +700,11 @@
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -653,8 +714,11 @@
       <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -664,8 +728,11 @@
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -675,8 +742,11 @@
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -686,8 +756,11 @@
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -697,8 +770,11 @@
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -708,8 +784,11 @@
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -719,8 +798,11 @@
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -730,8 +812,11 @@
       <c r="C24" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -741,8 +826,11 @@
       <c r="C25" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -752,8 +840,11 @@
       <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -763,8 +854,11 @@
       <c r="C27" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -774,8 +868,11 @@
       <c r="C28" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -785,8 +882,11 @@
       <c r="C29" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -796,8 +896,11 @@
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -807,8 +910,11 @@
       <c r="C31" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -818,8 +924,11 @@
       <c r="C32" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -829,8 +938,11 @@
       <c r="C33" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -840,8 +952,11 @@
       <c r="C34" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -851,8 +966,11 @@
       <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -862,8 +980,11 @@
       <c r="C36" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -873,8 +994,11 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -884,8 +1008,11 @@
       <c r="C38" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -895,8 +1022,11 @@
       <c r="C39" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -906,8 +1036,11 @@
       <c r="C40" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -917,8 +1050,11 @@
       <c r="C41" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -928,8 +1064,11 @@
       <c r="C42" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -939,8 +1078,11 @@
       <c r="C43" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -950,8 +1092,11 @@
       <c r="C44" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -961,8 +1106,11 @@
       <c r="C45" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -972,8 +1120,11 @@
       <c r="C46" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -983,8 +1134,11 @@
       <c r="C47" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -4398,6 +4552,11 @@
       <c r="C536" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{EF3F8763-9D6A-4892-9D5B-2880E4DCD2D3}"/>
+    <hyperlink ref="D3:D47" r:id="rId2" display="https://www.cleverbot.com/conv/202202041647/WYDS891QFL_Hello-who-are-you" xr:uid="{D066D253-BAFC-47E1-B14B-5CD6F4999E59}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying a different filter model for the search_box
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD92217-9AEA-4741-8B04-5D676C213A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEC8344-6B7D-43AA-9211-00D3ED716BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="-25356" yWindow="2292" windowWidth="22344" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="23">
   <si>
     <t>Kanal</t>
   </si>
@@ -77,6 +77,34 @@
   </si>
   <si>
     <t>https://www.cleverbot.com/conv/202202051853/AYAIFK7NLP_What-is-your-favourite-word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Do you have any book recommendations?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I don't know.</t>
+  </si>
+  <si>
+    <t>asfd</t>
+  </si>
+  <si>
+    <t>afer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Can you guess what number I am thinking of?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+4?</t>
+  </si>
+  <si>
+    <t>hgaehtr</t>
+  </si>
+  <si>
+    <t>ahergfae</t>
   </si>
 </sst>
 </file>
@@ -461,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
   <dimension ref="A1:H536"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,7 +531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -516,6 +544,18 @@
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -531,7 +571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,7 +584,18 @@
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
cleverbot live conversation implemented
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64019560-A39F-4E17-957E-19438B4766AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AC5D68-66C5-434E-A599-05A047595C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28128" yWindow="2304" windowWidth="22344" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="18">
   <si>
     <t>Kanal</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>https://www.cleverbot.com/conv/202202071112/WYBQYLD7AN_Good-day</t>
+  </si>
+  <si>
+    <t>https://www.cleverbot.com/conv/202202071608/WXBLHBYZ88_Hello-there</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
-  <dimension ref="A1:H536"/>
+  <dimension ref="A1:H537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -534,23 +537,22 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -563,35 +565,36 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1154,7 +1157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
@@ -1163,6 +1166,9 @@
       </c>
       <c r="C48" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -3828,12 +3834,20 @@
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A291" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C291" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C292" s="3"/>
+      <c r="C292" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C293" s="3"/>
@@ -4567,14 +4581,17 @@
     <row r="536" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C536" s="3"/>
     </row>
+    <row r="537" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C537" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{7D37BC6F-574B-4B5A-9EEF-CCF688CE2483}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{E753D133-491A-42F3-938E-56B985B734AF}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{E227330E-1499-418E-87D7-5D6F0C09E101}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{7D37BC6F-574B-4B5A-9EEF-CCF688CE2483}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{E753D133-491A-42F3-938E-56B985B734AF}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{E227330E-1499-418E-87D7-5D6F0C09E101}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{D742725B-5690-4704-8C5C-B5F2B019D055}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{0686292A-70BB-4C00-985A-CD546531B6FB}"/>
-    <hyperlink ref="D6" r:id="rId6" xr:uid="{7DD1934C-481D-4BFA-A2C1-AD1AD03B8DF4}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{0686292A-70BB-4C00-985A-CD546531B6FB}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{7DD1934C-481D-4BFA-A2C1-AD1AD03B8DF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
auto email + phone number highlighting implemented
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E316AA52-C593-4704-BA37-F8D3CB52A471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B197EC7-5499-424E-A196-F2224B4FA997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="18">
   <si>
     <t>Kanal</t>
   </si>
@@ -86,52 +86,6 @@
   </si>
   <si>
     <t>https://www.cleverbot.com/conv/202202071608/WXBLHBYZ88_Hello-there</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I am doing well. Can you tell me a joke?
-How about a story then?
-Yes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-How are you doing today?
-No I don't know any jokes.
-You want me to tell you a story?
-Once upon a time, ***.</t>
-  </si>
-  <si>
-    <t>Ja, der Bot konnte das Anliegen jedoch nicht selbst lösen.</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The Turing test, originally called the imitation game by Alan Turing in 1950, is a test of a machine's ability to exhibit intelligent behaviour equivalent to, or indistinguishable from, that of a huma.
-I am doing pretty well. But then again I am probably like an 8 or 9 on the alive scale.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-No, what is that?
-Yes I am fine how about you?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Good day!
-It has its ups and downs.
-I am well, thank you.
-I am not sure, but it must be a lot.
-I was born at a very young age. A long long time ago.
-How have you been faring since then?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-How are you on this fine day?
-How many times have you blinked today?
-When do you think you were created?
-As was I.
-Great, and you?</t>
   </si>
 </sst>
 </file>
@@ -522,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
   <dimension ref="A1:H537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +486,8 @@
     <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="69.77734375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="21.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31.77734375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="29.21875" style="5" customWidth="1"/>
     <col min="8" max="8" width="18.77734375" style="5" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="5"/>
@@ -564,7 +519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -577,20 +532,10 @@
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -603,12 +548,6 @@
       <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
@@ -624,12 +563,6 @@
       </c>
       <c r="D4" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
analysis multi threading implemented
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E92946-A1E6-47C0-9A55-1466C1DB19D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCFDF9A-0475-4DA3-8923-4EE5815D767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="22">
   <si>
     <t>Kanal</t>
   </si>
@@ -86,6 +86,28 @@
   </si>
   <si>
     <t>https://www.cleverbot.com/conv/202202071608/WXBLHBYZ88_Hello-there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Any movie.
+Hulk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Sure. What movie.
+Superman or hulk?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I am cleverbot.
+What is your name?
+42.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Why do you want to know my name?
+What is the question to life, the universe, and everything?
+What is the question to life, the universe and everything?</t>
   </si>
 </sst>
 </file>
@@ -476,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
   <dimension ref="A1:H537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -580,7 +602,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -593,8 +615,14 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,7 +635,12 @@
       <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">

</xml_diff>

<commit_message>
Auto highlighting working. auto anonymizing is not
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCFDF9A-0475-4DA3-8923-4EE5815D767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76D270-BF91-478C-B4B8-F59DA381304F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="24">
   <si>
     <t>Kanal</t>
   </si>
@@ -108,6 +108,14 @@
 Why do you want to know my name?
 What is the question to life, the universe, and everything?
 What is the question to life, the universe and everything?</t>
+  </si>
+  <si>
+    <t>https://www.cleverbot.com/conv/202202140855/WXB9GR35ZN_Hey-can-I-tell-you-my-phone-number-it-is-0782315465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hey, can I tell you my phone number? it is 0782315465.
+Certainly. 0797781232</t>
   </si>
 </sst>
 </file>
@@ -498,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
   <dimension ref="A1:H537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,7 +678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -681,7 +689,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4637,8 +4648,9 @@
     <hyperlink ref="D8" r:id="rId4" xr:uid="{0686292A-70BB-4C00-985A-CD546531B6FB}"/>
     <hyperlink ref="D7" r:id="rId5" xr:uid="{F9CEFC09-4B00-4E96-9060-44420F1B18A4}"/>
     <hyperlink ref="D4" r:id="rId6" xr:uid="{14EFC6E9-6CC0-4BCF-A8AA-9E87E8724604}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{8BE5269C-7A6F-4A45-A714-A6DA224CB9EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preparing to make multiline QTableView editors
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3264D361-2689-4792-B214-932EFC7B378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733BF31C-E099-44E4-8C8B-0D375813ED2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="948" windowWidth="22104" windowHeight="12252" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="948" windowWidth="22104" windowHeight="12252" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
pandasgui show event resizeRowsToContents impl
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733BF31C-E099-44E4-8C8B-0D375813ED2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B37422-F16B-4AF0-A218-D761BD0359CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="0" yWindow="948" windowWidth="22104" windowHeight="12252" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="35">
   <si>
     <t>Kanal</t>
   </si>
@@ -124,28 +124,72 @@
     <t>asgfd</t>
   </si>
   <si>
-    <t>Hello there.
+    <t>asdfhihb asdnfoinawpef hbad</t>
+  </si>
+  <si>
+    <t>Hi there.
+Very well. What happened next?
+That's so sad. How did it happen?
+Tragic. Why did they have it out for you?
+The other side of what?
+So you do have jokes!
+I am doing well. Can you tell me a joke?
+How about a story then?
+Yes.
+What was the pony's name?</t>
+  </si>
+  <si>
+    <t>How are you doing today?
+He died.
+An explosion that was meant to kill me.
+To get to get to the other side.
+The other side of the road!
+No I don't know any jokes.
+You want me to tell you a story?
+Once upon a time, there was a pony.
+I didn't say pony, I said apple!</t>
+  </si>
+  <si>
+    <t>Have you ever heard of the Turing test?
+The Turing test, originally called the imitation game by Alan Turing in 1950, is a test of a machine's ability to exhibit intelligent behaviour equivalent to, or indistinguishable from, that of a huma.
 Are any of us answers?
 How alive would you say you are on a scale of 1 to 10?
 Are you ok?
 I am doing pretty well. But then again I am probably like an 8 or 9 on the alive scale.</t>
   </si>
   <si>
-    <t>How are you an answer?
-I think we are alive.
+    <t>I think we are alive.
 1.
-Yes I am fine how about you?</t>
+Yes I am fine how about you?
+Indeed.</t>
   </si>
   <si>
-    <t>asdfhihb asdnfoinawpef hbad</t>
+    <t>It has its ups and downs.
+I am not a web designer, but a friend of mine is a spider. Designs the best webs on the block.
+I am not sure, but it must be a lot.
+I was born at a very young age. A long long time ago.
+How have you been faring since then?</t>
   </si>
   <si>
-    <t>Hi there.
-I am doing well. Can you tell me a joke?</t>
+    <t>What do you like best about being a web designer?
+When do you think you were created?
+As was I.
+Great, and you?</t>
   </si>
   <si>
-    <t>How are you doing today?
-No I don't know any jokes.</t>
+    <t>What is your favourite word?
+What are you good at?
+Can I call you dude?
+Hey dude, how old are you?
+Can you guess what number I am thinking of?
+Close, it is actually 9.</t>
+  </si>
+  <si>
+    <t>My favorite word it 'dude'.
+Sure.
+1, I am a girl, 2, none of your business.
+4?
+I was never good at geography.</t>
   </si>
 </sst>
 </file>
@@ -588,7 +632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,10 +646,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>24</v>
@@ -614,7 +658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -628,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -651,8 +695,14 @@
       <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -664,6 +714,12 @@
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="6"/>
     </row>

</xml_diff>

<commit_message>
newlines are no longer being deleted in editor
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/transcripts.xlsx
+++ b/Content Engineer Studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AF4C9C-8755-4C8F-BA82-3E05ED08D787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FC8889-292B-46F1-8A5A-F66A0E3CF8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="8244" windowWidth="16368" windowHeight="6780" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="40">
   <si>
     <t>Kanal</t>
   </si>
@@ -111,32 +111,7 @@
     <t>Nein</t>
   </si>
   <si>
-    <t>Hey, can I tell you my super secret phone number? It is ***.
-How about my email? It is ***
-Do you have an email address?</t>
-  </si>
-  <si>
-    <t>You can tell me anything.
-What about them?</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nam hendrerit, ligula ut ullamcorper volutpat, tortor massa rutrum sem, vitae fringilla arcu nisl in odio.</t>
-  </si>
-  <si>
     <t>Ja</t>
-  </si>
-  <si>
-    <t>Hi there.
-I am doing well. Can you tell me a joke?
-How about a story then?
-Yes.
-What was the pony's name?</t>
-  </si>
-  <si>
-    <t>How are you doing today?
-No I don't know any jokes.
-You want me to tell you a story?
-Once upon a time, there was a pony.</t>
   </si>
   <si>
     <t>In felis ipsum, sagittis nec porta convallis, tristique ut arcu. Maecenas vitae sodales ligula, auctor gravida ligula. Donec eu accumsan quam. Nullam dictum orci eros,</t>
@@ -195,6 +170,20 @@
   </si>
   <si>
     <t>Vivamus ultricies lacinia lectus, nec consequat magna scelerisque et. Duis nec elementum elit. Nunc sem tellus, faucibus et efficitur at, posuere at est. Cras dignis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit.
+Nam hendrerit, ligula ut ullamcorper volutpat, tortor
+massa rutrum sem, vitae fringilla arcu nisl in odio.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whatsapp
+asdfhi
+aisufdhg
+end
+asdfiug
+</t>
   </si>
 </sst>
 </file>
@@ -595,7 +584,7 @@
   <dimension ref="A1:O538"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,9 +626,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -650,17 +639,11 @@
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
@@ -676,17 +659,13 @@
       <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -710,14 +689,14 @@
         <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -767,13 +746,13 @@
         <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>23</v>
@@ -793,16 +772,16 @@
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
@@ -819,16 +798,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>